<commit_message>
fixing up building id
</commit_message>
<xml_diff>
--- a/database/import_from_excel/All_Buildings_All_Units.xlsx
+++ b/database/import_from_excel/All_Buildings_All_Units.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koschmann\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bospo\source\repos\das\plymouth-housing\database\import_from_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CFC5DE5-897F-483A-B886-853E3AB77F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5508CCF-6386-445D-A62A-B261E9FE716F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{FDB8C02D-EE2D-40A7-87D1-404303298A90}"/>
+    <workbookView xWindow="2955" yWindow="1950" windowWidth="21600" windowHeight="12645" xr2:uid="{FDB8C02D-EE2D-40A7-87D1-404303298A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>PST</t>
   </si>
   <si>
-    <t>SGOLEW</t>
-  </si>
-  <si>
     <t>SIM</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>1-720</t>
+  </si>
+  <si>
+    <t>SGO/LEW</t>
   </si>
 </sst>
 </file>
@@ -920,12 +920,12 @@
   <dimension ref="A1:N265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -954,19 +954,19 @@
         <v>8</v>
       </c>
       <c r="J1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="22" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
         <v>201</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5">
         <v>201</v>
@@ -1021,7 +1021,7 @@
         <v>202</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5">
         <v>202</v>
@@ -1065,7 +1065,7 @@
         <v>203</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5">
         <v>203</v>
@@ -1109,7 +1109,7 @@
         <v>204</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5">
         <v>204</v>
@@ -1153,7 +1153,7 @@
         <v>205</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5">
         <v>205</v>
@@ -1197,7 +1197,7 @@
         <v>206</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5">
         <v>206</v>
@@ -1241,7 +1241,7 @@
         <v>207</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="5">
         <v>207</v>
@@ -1285,7 +1285,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5">
         <v>208</v>
@@ -1329,7 +1329,7 @@
         <v>209</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5">
         <v>209</v>
@@ -1373,7 +1373,7 @@
         <v>210</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="5">
         <v>210</v>
@@ -1417,7 +1417,7 @@
         <v>211</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5">
         <v>211</v>
@@ -1461,7 +1461,7 @@
         <v>212</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5">
         <v>212</v>
@@ -1505,7 +1505,7 @@
         <v>213</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5">
         <v>213</v>
@@ -1549,7 +1549,7 @@
         <v>214</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5">
         <v>214</v>
@@ -1593,7 +1593,7 @@
         <v>215</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5">
         <v>215</v>
@@ -1637,7 +1637,7 @@
         <v>216</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5">
         <v>301</v>
@@ -1681,7 +1681,7 @@
         <v>217</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5">
         <v>302</v>
@@ -1725,7 +1725,7 @@
         <v>218</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5">
         <v>303</v>
@@ -1769,7 +1769,7 @@
         <v>219</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="5">
         <v>304</v>
@@ -1813,7 +1813,7 @@
         <v>220</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="5">
         <v>305</v>
@@ -1857,7 +1857,7 @@
         <v>221</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="5">
         <v>306</v>
@@ -1901,7 +1901,7 @@
         <v>222</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="5">
         <v>307</v>
@@ -1945,7 +1945,7 @@
         <v>223</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="5">
         <v>308</v>
@@ -1989,7 +1989,7 @@
         <v>225</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="5">
         <v>309</v>
@@ -2033,7 +2033,7 @@
         <v>226</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="5">
         <v>310</v>
@@ -2077,7 +2077,7 @@
         <v>227</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="5">
         <v>311</v>
@@ -2121,7 +2121,7 @@
         <v>228</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="5">
         <v>312</v>
@@ -2165,7 +2165,7 @@
         <v>229</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="5">
         <v>313</v>
@@ -2209,7 +2209,7 @@
         <v>301</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="5">
         <v>314</v>
@@ -2253,7 +2253,7 @@
         <v>302</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="5">
         <v>315</v>
@@ -2297,7 +2297,7 @@
         <v>303</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5">
         <v>401</v>
@@ -2341,7 +2341,7 @@
         <v>304</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="5">
         <v>402</v>
@@ -2385,7 +2385,7 @@
         <v>305</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="5">
         <v>403</v>
@@ -2429,7 +2429,7 @@
         <v>306</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="5">
         <v>404</v>
@@ -2473,7 +2473,7 @@
         <v>307</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="5">
         <v>405</v>
@@ -2517,7 +2517,7 @@
         <v>308</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="5">
         <v>406</v>
@@ -2561,7 +2561,7 @@
         <v>309</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="5">
         <v>407</v>
@@ -2605,7 +2605,7 @@
         <v>310</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="5">
         <v>408</v>
@@ -2649,7 +2649,7 @@
         <v>311</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="5">
         <v>409</v>
@@ -2693,7 +2693,7 @@
         <v>312</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="5">
         <v>410</v>
@@ -2737,7 +2737,7 @@
         <v>313</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" s="5">
         <v>411</v>
@@ -2781,7 +2781,7 @@
         <v>314</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" s="5">
         <v>412</v>
@@ -2825,7 +2825,7 @@
         <v>315</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" s="5">
         <v>413</v>
@@ -2869,7 +2869,7 @@
         <v>316</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="5">
         <v>414</v>
@@ -2913,7 +2913,7 @@
         <v>317</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" s="5">
         <v>415</v>
@@ -2957,7 +2957,7 @@
         <v>318</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="5">
         <v>501</v>
@@ -3001,7 +3001,7 @@
         <v>319</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="5">
         <v>502</v>
@@ -3045,7 +3045,7 @@
         <v>320</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="5">
         <v>503</v>
@@ -3089,7 +3089,7 @@
         <v>321</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D50" s="5">
         <v>504</v>
@@ -3133,7 +3133,7 @@
         <v>322</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D51" s="5">
         <v>505</v>
@@ -3177,7 +3177,7 @@
         <v>323</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52" s="5">
         <v>506</v>
@@ -3221,7 +3221,7 @@
         <v>324</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D53" s="5">
         <v>507</v>
@@ -3265,7 +3265,7 @@
         <v>325</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" s="5">
         <v>508</v>
@@ -3309,7 +3309,7 @@
         <v>327</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D55" s="5">
         <v>509</v>
@@ -3353,7 +3353,7 @@
         <v>328</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D56" s="5">
         <v>510</v>
@@ -3397,7 +3397,7 @@
         <v>329</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D57" s="5">
         <v>511</v>
@@ -3441,7 +3441,7 @@
         <v>401</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D58" s="5">
         <v>512</v>
@@ -3485,7 +3485,7 @@
         <v>402</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59" s="5">
         <v>513</v>
@@ -3529,7 +3529,7 @@
         <v>403</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" s="5">
         <v>514</v>
@@ -3573,7 +3573,7 @@
         <v>404</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D61" s="5">
         <v>515</v>
@@ -3617,7 +3617,7 @@
         <v>405</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D62" s="5">
         <v>601</v>
@@ -3661,7 +3661,7 @@
         <v>406</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D63" s="5">
         <v>602</v>
@@ -3705,7 +3705,7 @@
         <v>407</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D64" s="5">
         <v>603</v>
@@ -3749,7 +3749,7 @@
         <v>408</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D65" s="5">
         <v>604</v>
@@ -3793,7 +3793,7 @@
         <v>409</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D66" s="5">
         <v>605</v>
@@ -3835,7 +3835,7 @@
         <v>410</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="5">
         <v>606</v>
@@ -3877,7 +3877,7 @@
         <v>411</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" s="5">
         <v>607</v>
@@ -3919,7 +3919,7 @@
         <v>412</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D69" s="5">
         <v>608</v>
@@ -3961,7 +3961,7 @@
         <v>413</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D70" s="5">
         <v>609</v>
@@ -4003,7 +4003,7 @@
         <v>414</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D71" s="5">
         <v>610</v>
@@ -4045,7 +4045,7 @@
         <v>415</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D72" s="5">
         <v>611</v>
@@ -4085,7 +4085,7 @@
         <v>416</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D73" s="5">
         <v>612</v>
@@ -4125,7 +4125,7 @@
         <v>417</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D74" s="5">
         <v>613</v>
@@ -4165,7 +4165,7 @@
         <v>418</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D75" s="5">
         <v>614</v>
@@ -4205,7 +4205,7 @@
         <v>419</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D76" s="5">
         <v>615</v>
@@ -4245,7 +4245,7 @@
         <v>420</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D77" s="5">
         <v>701</v>
@@ -4285,7 +4285,7 @@
         <v>421</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D78" s="5">
         <v>702</v>
@@ -4325,7 +4325,7 @@
         <v>422</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D79" s="5">
         <v>703</v>
@@ -4337,7 +4337,7 @@
         <v>420</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="8">
@@ -4365,7 +4365,7 @@
         <v>423</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D80" s="5">
         <v>704</v>
@@ -4377,7 +4377,7 @@
         <v>421</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="8">
@@ -4405,7 +4405,7 @@
         <v>424</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D81" s="5">
         <v>708</v>
@@ -4417,7 +4417,7 @@
         <v>422</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="8">
@@ -4445,7 +4445,7 @@
         <v>425</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D82" s="5">
         <v>712</v>
@@ -4457,7 +4457,7 @@
         <v>423</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="8">
@@ -4485,7 +4485,7 @@
         <v>427</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D83" s="5">
         <v>713</v>
@@ -4497,7 +4497,7 @@
         <v>424</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="8">
@@ -4522,7 +4522,7 @@
         <v>428</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D84" s="5">
         <v>714</v>
@@ -4534,7 +4534,7 @@
         <v>425</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="8">
@@ -4556,7 +4556,7 @@
         <v>429</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D85" s="9">
         <v>715</v>
@@ -4568,7 +4568,7 @@
         <v>426</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="10">
@@ -4590,7 +4590,7 @@
         <v>501</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E86" s="5">
         <v>711</v>
@@ -4599,7 +4599,7 @@
         <v>427</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -4619,7 +4619,7 @@
         <v>502</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E87" s="5">
         <v>712</v>
@@ -4628,7 +4628,7 @@
         <v>428</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -4648,7 +4648,7 @@
         <v>503</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E88" s="5">
         <v>713</v>
@@ -4657,7 +4657,7 @@
         <v>429</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -4677,7 +4677,7 @@
         <v>504</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E89" s="5">
         <v>714</v>
@@ -4686,7 +4686,7 @@
         <v>430</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -4706,7 +4706,7 @@
         <v>505</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E90" s="5">
         <v>715</v>
@@ -4715,7 +4715,7 @@
         <v>431</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -4735,7 +4735,7 @@
         <v>506</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E91" s="5">
         <v>716</v>
@@ -4744,7 +4744,7 @@
         <v>432</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -4764,7 +4764,7 @@
         <v>507</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E92" s="9">
         <v>717</v>
@@ -4773,7 +4773,7 @@
         <v>433</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -4793,13 +4793,13 @@
         <v>508</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F93" s="11">
         <v>434</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
@@ -4819,10 +4819,10 @@
         <v>509</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -4839,10 +4839,10 @@
         <v>510</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
@@ -4859,10 +4859,10 @@
         <v>511</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
@@ -4879,10 +4879,10 @@
         <v>512</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
@@ -4899,10 +4899,10 @@
         <v>513</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
@@ -4919,10 +4919,10 @@
         <v>514</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
@@ -4939,10 +4939,10 @@
         <v>515</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
@@ -4959,10 +4959,10 @@
         <v>516</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
@@ -4980,7 +4980,7 @@
       </c>
       <c r="C102" s="13"/>
       <c r="G102" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="C103" s="13"/>
       <c r="G103" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>

</xml_diff>